<commit_message>
bar menu update with cl
</commit_message>
<xml_diff>
--- a/functions/menus/bardrinks.xlsx
+++ b/functions/menus/bardrinks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aknar\Documents\GitHub\mall-restaurant\functions\menus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\URBANFOODCOURT1\Users\FC1\OneDrive\Documents\mall-restaurant\functions\menus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E2D2235-744B-4E0E-A50A-3A99906D432C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E681D47F-4156-4E78-8F24-2ED20C03C5F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{9368492B-7E17-47C5-A814-03528FA33168}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9368492B-7E17-47C5-A814-03528FA33168}"/>
   </bookViews>
   <sheets>
     <sheet name="FOR THE TEETOTALLERS" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="BEER" sheetId="6" r:id="rId6"/>
     <sheet name="WHISKY" sheetId="7" r:id="rId7"/>
     <sheet name="SCOTCH" sheetId="8" r:id="rId8"/>
+    <sheet name="Bottle" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
   <si>
     <t>MINERAL WATER (1 LTR.)</t>
   </si>
@@ -263,6 +264,21 @@
   </si>
   <si>
     <t>CAMINO 30 ml</t>
+  </si>
+  <si>
+    <t>Whisky</t>
+  </si>
+  <si>
+    <t>Rum</t>
+  </si>
+  <si>
+    <t>Scotch</t>
+  </si>
+  <si>
+    <t>Vodka</t>
+  </si>
+  <si>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -626,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09536465-D12A-4950-8B53-9E1B98592CF7}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +756,14 @@
       </c>
       <c r="B13" s="1">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1230,12 +1254,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C09325-F95E-4D8A-B4B9-597B9400116F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1432,4 +1457,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0EC1BC-BFF3-4B39-BD8F-5C6B8BAB862D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5">
+        <v>1600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>